<commit_message>
Primer intento de lectura y escritura en Unity3D
Lectura de archivo externo en formato xml editado desde un archivo .xlxs
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -26,22 +26,25 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{EC4F1CE8-C818-4B4A-9C73-F4EDE8275A5C}" name="data-set.schema" type="4" refreshedVersion="0" background="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="data-set.schema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ironh\Desktop\data-set.schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" xr16:uid="{5A86D468-51A7-48ED-AE54-A78E1106DCF5}" name="data-set.schema1" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="data-set.schema1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ironh\Desktop\data-set.schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" xr16:uid="{980DF187-4075-49FF-A3AE-34A12CA9C4B2}" name="data-set.schema2" type="4" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="data-set.schema2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ironh\Desktop\data-set.schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="4" xr16:uid="{7084B746-73FB-4AD8-9DD8-07ECB2449B64}" name="data-set.schema3" type="4" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="data-set.schema3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ironh\Desktop\data-set.schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" xr16:uid="{65C17C8F-0346-4824-8AA0-F3002400D65B}" name="data-set.schema4" type="4" refreshedVersion="0" background="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="data-set.schema4" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ironh\Desktop\data-set.schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" xr16:uid="{7428FCB1-0FAA-4487-9645-F8E70F791F73}" name="test001Xml" type="4" refreshedVersion="0" background="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="test001Xml" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\ironh\Documents\DataManagerExample\Assets\test001Xml.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="7" xr16:uid="{CA41A9DF-FC64-4FE5-9C6F-6857B3DBDE93}" name="test001Xml1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ironh\Documents\DataManagerExample\Assets\test001Xml.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -196,7 +199,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema6">
+  <Schema ID="Schema2">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="DataPool">
         <xsd:complexType>
@@ -208,6 +211,11 @@
                     <xsd:complexType>
                       <xsd:sequence minOccurs="0">
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RawMaterial1" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RawMaterial2" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RawMaterial3" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Quantity1" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Quantity2" form="unqualified"/>
+                        <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="Quantity3" form="unqualified"/>
                         <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="NodeID" form="unqualified"/>
                       </xsd:sequence>
                     </xsd:complexType>
@@ -220,27 +228,35 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="6" Name="DataPool_Map" RootElement="DataPool" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="6" DataBindingLoadMode="1"/>
+  <Map ID="7" Name="DataPool_Map" RootElement="DataPool" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="7" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{D62F827F-A45D-4258-B223-BCFD5C9E63A2}" name="Table24" displayName="Table24" ref="A1:G5" tableType="xml" totalsRowShown="0" headerRowDxfId="0" connectionId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{D62F827F-A45D-4258-B223-BCFD5C9E63A2}" name="Table24" displayName="Table24" ref="A1:G5" tableType="xml" totalsRowShown="0" headerRowDxfId="0" connectionId="7">
   <autoFilter ref="A1:G5" xr:uid="{AE6796BC-09AB-43B7-BC4B-F7161E40181E}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6170FEF0-C8F1-4E93-976C-9272447DAB1B}" uniqueName="NodeID" name="NodeID">
-      <xmlColumnPr mapId="6" xpath="/DataPool/Nodes/Node/NodeID" xmlDataType="string"/>
+      <xmlColumnPr mapId="7" xpath="/DataPool/Nodes/Node/NodeID" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{F99864A9-945F-432C-B4B7-64D2EA5FD80F}" uniqueName="RawMaterial1" name="RawMaterial1">
-      <xmlColumnPr mapId="6" xpath="/DataPool/Nodes/Node/RawMaterial1" xmlDataType="string"/>
+      <xmlColumnPr mapId="7" xpath="/DataPool/Nodes/Node/RawMaterial1" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{34BD1530-76BA-4075-A82D-C1414BA7988F}" uniqueName="cant1" name="cant1"/>
-    <tableColumn id="4" xr3:uid="{55A5E4D1-AD97-4AE4-BABD-BE598C031DDD}" uniqueName="RawMaterial2" name="RawMaterial2"/>
-    <tableColumn id="5" xr3:uid="{B8EAA5BD-ED67-4DAB-A9E8-30D855FF3BD3}" uniqueName="cant2" name="cant2"/>
-    <tableColumn id="6" xr3:uid="{41D030AB-0926-4698-8E10-1FBCE58EF45D}" uniqueName="RawMaterial3" name="RawMaterial3"/>
-    <tableColumn id="7" xr3:uid="{234D90B4-1BA8-4553-BE97-38D1990E6309}" uniqueName="cant3" name="cant3"/>
+    <tableColumn id="3" xr3:uid="{34BD1530-76BA-4075-A82D-C1414BA7988F}" uniqueName="Quantity1" name="cant1">
+      <xmlColumnPr mapId="7" xpath="/DataPool/Nodes/Node/Quantity1" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{55A5E4D1-AD97-4AE4-BABD-BE598C031DDD}" uniqueName="RawMaterial2" name="RawMaterial2">
+      <xmlColumnPr mapId="7" xpath="/DataPool/Nodes/Node/RawMaterial2" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B8EAA5BD-ED67-4DAB-A9E8-30D855FF3BD3}" uniqueName="Quantity2" name="cant2">
+      <xmlColumnPr mapId="7" xpath="/DataPool/Nodes/Node/Quantity2" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{41D030AB-0926-4698-8E10-1FBCE58EF45D}" uniqueName="RawMaterial3" name="RawMaterial3">
+      <xmlColumnPr mapId="7" xpath="/DataPool/Nodes/Node/RawMaterial3" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{234D90B4-1BA8-4553-BE97-38D1990E6309}" uniqueName="Quantity3" name="cant3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -561,7 +577,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>